<commit_message>
últimos cambios en el servidor SVN
</commit_message>
<xml_diff>
--- a/src/main/resources/plantillas/nomina/Historial_Pago.xlsx
+++ b/src/main/resources/plantillas/nomina/Historial_Pago.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo Mex\Dropbox\folf\siayf-rh\Reportes\luis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo Mex\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="20490" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="Historial_Pago" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>R. F. C.</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>62 PENSIÓN ALIMENTICIA</t>
+  </si>
+  <si>
+    <t>NOMBRE PRODUCTO</t>
+  </si>
+  <si>
+    <t>INICIO PERIODO</t>
+  </si>
+  <si>
+    <t>FIN PERIODO</t>
   </si>
 </sst>
 </file>
@@ -111,7 +120,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +142,14 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -188,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -208,6 +225,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -489,114 +513,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="J1" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1:Z1048576"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="8"/>
-    <col min="13" max="13" width="19.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="8"/>
-    <col min="19" max="19" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8" style="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="8"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="14" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="8"/>
+    <col min="16" max="16" width="19.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="8"/>
+    <col min="22" max="22" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21" style="8" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:29" s="1" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>